<commit_message>
adding EDA on no-diet people
</commit_message>
<xml_diff>
--- a/Exploratory Data Analysis/formated_table_one.xlsx
+++ b/Exploratory Data Analysis/formated_table_one.xlsx
@@ -1,34 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AltanGadasTbl\R_file\nhanes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AltanGadasTbl\Documents\ENAR-DataFest\Exploratory Data Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C52AE4-B0C1-4834-BB33-756FDCB806DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBEA4E9A-8370-4B6B-8277-9C03FBB5A51B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D6783829-0EF3-4BFC-81B2-C15EC00B51FB}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D6783829-0EF3-4BFC-81B2-C15EC00B51FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>18 to 44</t>
   </si>
@@ -152,8 +158,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="176" formatCode="0.000%"/>
+    <numFmt numFmtId="180" formatCode="0.000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -242,7 +249,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -273,83 +280,62 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -367,22 +353,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="table_one"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -682,10 +652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D727581A-4AC4-4796-9617-6267BB58CEAF}">
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:J52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -714,41 +684,41 @@
       <c r="E1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="F1" s="7" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="25" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C2" s="9">
-        <f>SUM(D2:E2)</f>
+        <f>D2+E2</f>
         <v>0.242207347451907</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="9">
         <v>0.13381980726861101</v>
       </c>
       <c r="E2" s="4">
         <v>0.10838754018329599</v>
       </c>
-      <c r="F2" t="s">
-        <v>33</v>
+      <c r="F2" s="28">
+        <v>0.60152077984101204</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="10"/>
+      <c r="A3" s="25"/>
       <c r="B3" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="9">
-        <f t="shared" ref="C3:C5" si="0">SUM(D3:E3)</f>
+        <f t="shared" ref="C3:C5" si="0">D3+E3</f>
         <v>0.24806624482767498</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="9">
         <v>0.140988090548826</v>
       </c>
       <c r="E3" s="4">
@@ -756,7 +726,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="10"/>
+      <c r="A4" s="25"/>
       <c r="B4" s="1" t="s">
         <v>29</v>
       </c>
@@ -764,7 +734,7 @@
         <f t="shared" si="0"/>
         <v>0.25098946945185602</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="9">
         <v>0.13720001703138901</v>
       </c>
       <c r="E4" s="4">
@@ -772,7 +742,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="10"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="1" t="s">
         <v>30</v>
       </c>
@@ -780,7 +750,7 @@
         <f t="shared" si="0"/>
         <v>0.25873693826856203</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="9">
         <v>0.14308401681143501</v>
       </c>
       <c r="E5" s="4">
@@ -795,7 +765,7 @@
       <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="25" t="s">
         <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -816,7 +786,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="10"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
@@ -832,7 +802,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="10"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="1" t="s">
         <v>2</v>
       </c>
@@ -848,7 +818,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="10"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
@@ -871,7 +841,7 @@
       <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="25" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -892,7 +862,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="10"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="1" t="s">
         <v>5</v>
       </c>
@@ -915,104 +885,99 @@
       <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="22">
+      <c r="C15" s="9">
         <f t="shared" si="1"/>
         <v>0.15354603372966902</v>
       </c>
-      <c r="D15" s="23">
+      <c r="D15" s="15">
         <v>0.100787710550944</v>
       </c>
-      <c r="E15" s="23">
+      <c r="E15" s="15">
         <v>5.2758323178725003E-2</v>
       </c>
-      <c r="F15" s="24" t="s">
+      <c r="F15" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="21"/>
-      <c r="B16" s="18" t="s">
+      <c r="A16" s="25"/>
+      <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="22">
+      <c r="C16" s="9">
         <f t="shared" si="1"/>
         <v>5.5649748083311398E-2</v>
       </c>
-      <c r="D16" s="23">
+      <c r="D16" s="15">
         <v>3.48550960527352E-2</v>
       </c>
-      <c r="E16" s="23">
+      <c r="E16" s="15">
         <v>2.0794652030576202E-2</v>
       </c>
-      <c r="F16" s="24"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="21"/>
-      <c r="B17" s="18" t="s">
+      <c r="A17" s="25"/>
+      <c r="B17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="22">
+      <c r="C17" s="9">
         <f t="shared" si="1"/>
         <v>0.11528292996424619</v>
       </c>
-      <c r="D17" s="23">
+      <c r="D17" s="15">
         <v>5.4471818468068298E-2</v>
       </c>
-      <c r="E17" s="23">
+      <c r="E17" s="15">
         <v>6.0811111496177898E-2</v>
       </c>
-      <c r="F17" s="24"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="21"/>
-      <c r="B18" s="18" t="s">
+      <c r="A18" s="25"/>
+      <c r="B18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="22">
+      <c r="C18" s="9">
         <f t="shared" si="1"/>
         <v>0.64234926722276708</v>
       </c>
-      <c r="D18" s="23">
+      <c r="D18" s="15">
         <v>0.34631684854429701</v>
       </c>
-      <c r="E18" s="23">
+      <c r="E18" s="15">
         <v>0.29603241867847002</v>
       </c>
-      <c r="F18" s="24"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="21"/>
-      <c r="B19" s="18" t="s">
+      <c r="A19" s="25"/>
+      <c r="B19" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="22">
+      <c r="C19" s="9">
         <f t="shared" si="1"/>
         <v>3.3172021000005901E-2</v>
       </c>
-      <c r="D19" s="23">
+      <c r="D19" s="15">
         <v>1.8660458044215601E-2</v>
       </c>
-      <c r="E19" s="23">
+      <c r="E19" s="15">
         <v>1.45115629557903E-2</v>
       </c>
-      <c r="F19" s="24"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="32"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="24"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="25" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1033,7 +998,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="10"/>
+      <c r="A22" s="25"/>
       <c r="B22" s="1" t="s">
         <v>12</v>
       </c>
@@ -1049,7 +1014,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="10"/>
+      <c r="A23" s="25"/>
       <c r="B23" s="1" t="s">
         <v>13</v>
       </c>
@@ -1065,7 +1030,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="10"/>
+      <c r="A24" s="25"/>
       <c r="B24" s="1" t="s">
         <v>14</v>
       </c>
@@ -1088,42 +1053,42 @@
       <c r="E25" s="4"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="21" t="s">
+      <c r="A26" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="18" t="s">
+      <c r="B26" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="22">
+      <c r="C26" s="9">
         <f>D26+E26</f>
         <v>0.88903226086053</v>
       </c>
-      <c r="D26" s="23">
+      <c r="D26" s="15">
         <v>0.53078804660805101</v>
       </c>
-      <c r="E26" s="23">
+      <c r="E26" s="15">
         <v>0.35824421425247899</v>
       </c>
-      <c r="F26" s="24" t="s">
+      <c r="F26" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="25"/>
-      <c r="B27" s="26" t="s">
+      <c r="A27" s="26"/>
+      <c r="B27" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="27">
+      <c r="C27" s="17">
         <f>D27+E27</f>
         <v>0.11096773913947061</v>
       </c>
-      <c r="D27" s="28">
+      <c r="D27" s="18">
         <v>2.4303885052209699E-2</v>
       </c>
-      <c r="E27" s="28">
+      <c r="E27" s="18">
         <v>8.6663854087260905E-2</v>
       </c>
-      <c r="F27" s="29"/>
+      <c r="F27" s="19"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="5"/>
@@ -1133,95 +1098,95 @@
       <c r="E28" s="4"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="14"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
+      <c r="A29" s="22"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="14"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
+      <c r="A30" s="22"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="12"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
+      <c r="A31" s="11"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="10"/>
-      <c r="B32" s="11"/>
+      <c r="A32" s="25"/>
+      <c r="B32" s="10"/>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
       <c r="E32" s="4"/>
-      <c r="F32" s="19"/>
+      <c r="F32" s="13"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" s="10"/>
-      <c r="B33" s="11"/>
+      <c r="A33" s="25"/>
+      <c r="B33" s="10"/>
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
       <c r="E33" s="4"/>
-      <c r="F33" s="19"/>
+      <c r="F33" s="13"/>
     </row>
     <row r="34" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="10"/>
-      <c r="B34" s="11"/>
+      <c r="A34" s="25"/>
+      <c r="B34" s="10"/>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
       <c r="E34" s="4"/>
-      <c r="F34" s="19"/>
+      <c r="F34" s="13"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35" s="10"/>
-      <c r="B35" s="11"/>
+      <c r="A35" s="25"/>
+      <c r="B35" s="10"/>
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
       <c r="E35" s="4"/>
-      <c r="F35" s="19"/>
+      <c r="F35" s="13"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="10"/>
-      <c r="B36" s="11"/>
+      <c r="A36" s="25"/>
+      <c r="B36" s="10"/>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
       <c r="E36" s="4"/>
-      <c r="F36" s="19"/>
+      <c r="F36" s="13"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A37" s="10"/>
-      <c r="B37" s="11"/>
+      <c r="A37" s="25"/>
+      <c r="B37" s="10"/>
       <c r="C37" s="9"/>
       <c r="D37" s="9"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="19"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="13"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A38" s="10"/>
-      <c r="B38" s="11"/>
+      <c r="A38" s="25"/>
+      <c r="B38" s="10"/>
       <c r="C38" s="9"/>
       <c r="D38" s="9"/>
       <c r="E38" s="4"/>
-      <c r="F38" s="19"/>
+      <c r="F38" s="13"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A39" s="12"/>
-      <c r="B39" s="15"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
+      <c r="A39" s="11"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A40" s="12"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
+      <c r="A40" s="11"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="5"/>
@@ -1231,94 +1196,80 @@
       <c r="E41" s="4"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A44" s="12"/>
+      <c r="A44" s="11"/>
       <c r="B44" s="6"/>
-      <c r="C44" s="13"/>
+      <c r="C44" s="12"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
     </row>
     <row r="45" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="21"/>
-      <c r="B45" s="30"/>
-      <c r="C45" s="31"/>
-      <c r="D45" s="17"/>
-      <c r="E45" s="17"/>
+      <c r="A45" s="25"/>
+      <c r="B45" s="20"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="24"/>
       <c r="I45" s="3"/>
       <c r="J45" s="3"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A46" s="21"/>
-      <c r="B46" s="30"/>
-      <c r="C46" s="31"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="17"/>
+      <c r="A46" s="25"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="24"/>
+      <c r="E46" s="24"/>
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A47" s="32"/>
-      <c r="B47" s="30"/>
-      <c r="C47" s="33"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
+      <c r="A47" s="5"/>
+      <c r="B47" s="20"/>
+      <c r="C47" s="21"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
       <c r="I47" s="3"/>
       <c r="J47" s="3"/>
     </row>
     <row r="48" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="14"/>
-      <c r="B48" s="15"/>
-      <c r="C48" s="16"/>
-      <c r="D48" s="17"/>
-      <c r="E48" s="17"/>
+      <c r="A48" s="22"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="23"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="24"/>
       <c r="I48" s="3"/>
       <c r="J48" s="3"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A49" s="14"/>
-      <c r="B49" s="15"/>
-      <c r="C49" s="16"/>
-      <c r="D49" s="17"/>
-      <c r="E49" s="17"/>
+      <c r="A49" s="22"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="24"/>
+      <c r="E49" s="24"/>
       <c r="I49" s="3"/>
       <c r="J49" s="3"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A50" s="34"/>
-      <c r="B50" s="24"/>
-      <c r="C50" s="24"/>
-      <c r="D50" s="24"/>
-      <c r="E50" s="24"/>
-    </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A51" s="14"/>
-      <c r="B51" s="15"/>
-      <c r="C51" s="16"/>
-      <c r="D51" s="17"/>
-      <c r="E51" s="17"/>
+      <c r="A51" s="22"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="23"/>
+      <c r="D51" s="24"/>
+      <c r="E51" s="24"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A52" s="14"/>
-      <c r="B52" s="15"/>
-      <c r="C52" s="16"/>
-      <c r="D52" s="17"/>
-      <c r="E52" s="17"/>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A53" s="34"/>
-      <c r="B53" s="24"/>
-      <c r="C53" s="24"/>
-      <c r="D53" s="24"/>
-      <c r="E53" s="24"/>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A54" s="34"/>
-      <c r="B54" s="24"/>
-      <c r="C54" s="24"/>
-      <c r="D54" s="24"/>
-      <c r="E54" s="24"/>
+      <c r="A52" s="22"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="23"/>
+      <c r="D52" s="24"/>
+      <c r="E52" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="A26:A27"/>
     <mergeCell ref="A51:A52"/>
     <mergeCell ref="C51:C52"/>
     <mergeCell ref="D51:D52"/>
@@ -1332,16 +1283,9 @@
     <mergeCell ref="E45:E46"/>
     <mergeCell ref="D48:D49"/>
     <mergeCell ref="E48:E49"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="A26:A27"/>
     <mergeCell ref="A45:A46"/>
     <mergeCell ref="A48:A49"/>
     <mergeCell ref="C45:C46"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="A2:A5"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>